<commit_message>
Finish StudentListLoad UI with confirmation dialog and model binding
</commit_message>
<xml_diff>
--- a/fr.istic.tools.scanexam/src/main/resources/mailing/mailMap.xlsx
+++ b/fr.istic.tools.scanexam/src/main/resources/mailing/mailMap.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Théo\git\ScanGrading\fr.istic.tools.scanexam\src\main\resources\mailing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FAB2C64-0522-4EE2-82BC-0BAB26201DD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF85FD4-ABFC-42F0-8779-D7C9C5D362FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="5430" windowWidth="28800" windowHeight="15435"/>
+    <workbookView xWindow="5430" yWindow="5430" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mailMap" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -882,11 +882,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,26 +895,27 @@
     <col min="2" max="2" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>